<commit_message>
Update Diagramme & Exportation Tâches
Update Diagramme & Exportation Tâches
</commit_message>
<xml_diff>
--- a/ressources/stockage/Diagramme-de-Gantt-sur-Excel-v3.xlsx
+++ b/ressources/stockage/Diagramme-de-Gantt-sur-Excel-v3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" tabRatio="670" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6930" tabRatio="670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Projet 1" sheetId="1" r:id="rId1"/>
@@ -4343,8 +4343,8 @@
   </sheetPr>
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="C24" workbookViewId="0">
+      <selection sqref="A1:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5602,7 +5602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>

</xml_diff>